<commit_message>
Linked farms to pasture objects
</commit_message>
<xml_diff>
--- a/sbp-abm/data/FarmsData.xlsx
+++ b/sbp-abm/data/FarmsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\sbp-abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AC58AC-49BB-4C00-896B-9D8C68578432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B355030F-850D-46C8-A782-2C8608FA17FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="60" windowWidth="9520" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>FARM_ID</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>Alcácer do Sal</t>
+  </si>
+  <si>
+    <t>Pasture</t>
+  </si>
+  <si>
+    <t>Natural Pasture</t>
+  </si>
+  <si>
+    <t>Sown Permanent Pasture</t>
   </si>
 </sst>
 </file>
@@ -584,19 +593,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.7265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,8 +616,11 @@
       <c r="C1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -617,8 +630,11 @@
       <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -628,8 +644,11 @@
       <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -639,8 +658,11 @@
       <c r="C4" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -650,8 +672,11 @@
       <c r="C5" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -661,8 +686,11 @@
       <c r="C6" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -672,8 +700,11 @@
       <c r="C7" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -683,8 +714,11 @@
       <c r="C8" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -694,8 +728,11 @@
       <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -705,8 +742,11 @@
       <c r="C10" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -716,8 +756,11 @@
       <c r="C11" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -727,8 +770,11 @@
       <c r="C12" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -738,8 +784,11 @@
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -749,8 +798,11 @@
       <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -760,8 +812,11 @@
       <c r="C15" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -771,8 +826,11 @@
       <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -782,8 +840,11 @@
       <c r="C17" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -793,8 +854,11 @@
       <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -804,8 +868,11 @@
       <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -815,8 +882,11 @@
       <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -826,8 +896,11 @@
       <c r="C21" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -837,8 +910,11 @@
       <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -848,8 +924,11 @@
       <c r="C23" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -859,8 +938,11 @@
       <c r="C24" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -870,8 +952,11 @@
       <c r="C25" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -881,8 +966,11 @@
       <c r="C26" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -892,8 +980,11 @@
       <c r="C27" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -903,8 +994,11 @@
       <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -914,8 +1008,11 @@
       <c r="C29" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -925,8 +1022,11 @@
       <c r="C30" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -936,8 +1036,11 @@
       <c r="C31" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -947,8 +1050,11 @@
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -958,8 +1064,11 @@
       <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -969,8 +1078,11 @@
       <c r="C34" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -980,8 +1092,11 @@
       <c r="C35" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -991,8 +1106,11 @@
       <c r="C36" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1002,8 +1120,11 @@
       <c r="C37" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1013,8 +1134,11 @@
       <c r="C38" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -1024,8 +1148,11 @@
       <c r="C39" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1035,8 +1162,11 @@
       <c r="C40" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -1046,8 +1176,11 @@
       <c r="C41" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -1057,8 +1190,11 @@
       <c r="C42" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -1067,6 +1203,9 @@
       </c>
       <c r="C43" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented step methods nested calling + calling to NPV calculation
</commit_message>
<xml_diff>
--- a/sbp-abm/data/FarmsData.xlsx
+++ b/sbp-abm/data/FarmsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\sbp-abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B355030F-850D-46C8-A782-2C8608FA17FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D63718D-1D95-4EEE-9996-D881F5CB185F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="60" windowWidth="9520" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -645,7 +645,7 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -673,7 +673,7 @@
         <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -701,7 +701,7 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -729,7 +729,7 @@
         <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -757,7 +757,7 @@
         <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -785,7 +785,7 @@
         <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -827,7 +827,7 @@
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -855,7 +855,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -911,7 +911,7 @@
         <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -939,7 +939,7 @@
         <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -967,7 +967,7 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -995,7 +995,7 @@
         <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1023,7 +1023,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1051,7 +1051,7 @@
         <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1079,7 +1079,7 @@
         <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1135,7 +1135,7 @@
         <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1163,7 +1163,7 @@
         <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1191,7 +1191,7 @@
         <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>